<commit_message>
add save and expenses groups
</commit_message>
<xml_diff>
--- a/Сентябрь_2023.xlsx
+++ b/Сентябрь_2023.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,33 +434,30 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>категория</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>сумма</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>комментарий</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Август month in progress
</commit_message>
<xml_diff>
--- a/Сентябрь_2023.xlsx
+++ b/Сентябрь_2023.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,92 +434,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>категория</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>сумма</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>комментарий</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>прочее</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>прочее</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>прочее</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>образование</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D6" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Half filled in Сентябрь_2023.xlsx
</commit_message>
<xml_diff>
--- a/Сентябрь_2023.xlsx
+++ b/Сентябрь_2023.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,17 +440,768 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>дата</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>категория</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>сумма</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>комментарий</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>45170</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>продукты</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>-80</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Магнит</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>01.09.2023</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>зарплата</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>40000</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>01.09.2023</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>квартплата</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>-15000</v>
+      </c>
+      <c r="D4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>01.09.2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>продукты</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>-940</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Перекресток</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>02.09.2023</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>транспорт</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>-470</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Метро</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>03.09.2023</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>транспорт</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>-39</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Urent</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>03.09.2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>транспорт</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>-54</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Urent</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>03.09.2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>развлечения</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>-200</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>MINI KOFEINYA</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>03.09.2023</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>развлечения</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>-200</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>MINI KOFEINYA</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>04.09.2023</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>развлечения</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>-175</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Молочный коктейль</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>04.09.2023</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>продукты</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>-710</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Перекресток</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>05.09.2023</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>продукты</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>-387</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Обед СМ</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>05.09.2023</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>продукты</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>-837</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Перекресток</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>06.09.2023</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>развлечения</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>-852</v>
+      </c>
+      <c r="D15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>06.09.2023</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>прочее</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>-220</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>OZON. Хомутики</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>06.09.2023</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>подработка</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>470</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Даша</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>06.09.2023</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>связь</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>-650</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Tele 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>06.09.2023</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>продукты</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>-335</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Обед Техноград</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>06.09.2023</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>транспорт</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>-470</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Метро</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>07.09.2023</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>здоровье</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>-1700</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>DDX fitness</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>07.09.2023</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>транспорт</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>-30</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Urent</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>07.09.2023</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>продукты</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>-72</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Перекресток</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>07.09.2023</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>здоровье</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>-321</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Зубная нить и леденцы</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>07.09.2023</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>продукты</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>-279</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Обед СМ</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>08.09.2023</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>транспорт</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>-300</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Тройка</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>09.09.2023</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>связь</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>-30</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Мегафон</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>09.09.2023</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>одежда</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>-6798</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Куртка и водолазка</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>10.09.2023</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>связь</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>-100</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Теле 2 раздача Wi-fi</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>11.09.2023</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>продукты</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>-332</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Перекресток</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>11.09.2023</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>продукты</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>-120</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Магнит</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>12.09.2023</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>продукты</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>-377</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Обед СМ</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>12.09.2023</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>продукты</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>-278</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Перекресток</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>13.09.2023</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>продукты</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>-281</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Обед СМ</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>14.09.2023</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>продукты</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>-390</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Обед СМ</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>15.09.2023</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>развлечения</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>-175</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Точка. Молочный коктель </t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>15.09.2023</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>одежда</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>-4005</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Рюкзак 13.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>17.09.2023</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>развлечения</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>-1400</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Хачипури</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>09.09.2023</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>подработка</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>5000</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Сборка ПК для Олега</t>
         </is>
       </c>
     </row>

</xml_diff>